<commit_message>
[2022 1] 0614 ADD : Last Report and document
</commit_message>
<xml_diff>
--- a/document/Gantt_Chart/8팀_Gantt_Chart.xlsx
+++ b/document/Gantt_Chart/8팀_Gantt_Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\다운로드 파일 임시 백업 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2022 1학기\01 학교 강의 관련 파일\05 종합설계프로젝트2\01 Code 관련\git\2022_Team_8_project\document\Gantt_Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1559DB21-EDCC-40F7-8F6C-94F73165892B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C62A87C-D19C-468E-B7F3-B0C9CA93C0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="93">
   <si>
     <t>프로젝트 이름</t>
   </si>
@@ -1959,7 +1959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2196,67 +2196,7 @@
     <xf numFmtId="0" fontId="45" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2269,7 +2209,70 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2639,20 +2642,19 @@
   </sheetPr>
   <dimension ref="A1:CE42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="9" max="15" width="3.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="68" width="3.42578125" customWidth="1"/>
+    <col min="9" max="68" width="3.42578125" customWidth="1"/>
     <col min="69" max="83" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2729,40 +2731,40 @@
     </row>
     <row r="2" spans="1:83" ht="41.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="89"/>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="89"/>
-      <c r="AE2" s="89"/>
-      <c r="AF2" s="89"/>
-      <c r="AG2" s="89"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="106"/>
+      <c r="X2" s="106"/>
+      <c r="Y2" s="106"/>
+      <c r="Z2" s="106"/>
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="106"/>
+      <c r="AC2" s="106"/>
+      <c r="AD2" s="106"/>
+      <c r="AE2" s="106"/>
+      <c r="AF2" s="106"/>
+      <c r="AG2" s="106"/>
       <c r="AH2" s="12"/>
       <c r="AI2" s="12"/>
       <c r="AJ2" s="12"/>
@@ -2873,41 +2875,41 @@
     </row>
     <row r="4" spans="1:83" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="97" t="s">
+      <c r="C4" s="101"/>
+      <c r="D4" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="94" t="s">
+      <c r="I4" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="95" t="s">
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
-      <c r="S4" s="92"/>
-      <c r="T4" s="92"/>
-      <c r="U4" s="92"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92"/>
-      <c r="X4" s="92"/>
-      <c r="Y4" s="92"/>
-      <c r="Z4" s="92"/>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="92"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="101"/>
+      <c r="S4" s="101"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="101"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="101"/>
+      <c r="X4" s="101"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="101"/>
+      <c r="AA4" s="101"/>
+      <c r="AB4" s="101"/>
       <c r="AC4" s="18"/>
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
@@ -2952,40 +2954,40 @@
     </row>
     <row r="5" spans="1:83" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="99" t="s">
+      <c r="C5" s="101"/>
+      <c r="D5" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
       <c r="H5" s="19"/>
-      <c r="I5" s="91" t="s">
+      <c r="I5" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="93">
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="108">
         <v>44622</v>
       </c>
-      <c r="Q5" s="92"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="92"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="92"/>
-      <c r="AA5" s="92"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="101"/>
+      <c r="S5" s="101"/>
+      <c r="T5" s="101"/>
+      <c r="U5" s="101"/>
+      <c r="V5" s="101"/>
+      <c r="W5" s="101"/>
+      <c r="X5" s="101"/>
+      <c r="Y5" s="101"/>
+      <c r="Z5" s="101"/>
+      <c r="AA5" s="101"/>
       <c r="AB5" s="20"/>
       <c r="AC5" s="18"/>
       <c r="AD5" s="1"/>
@@ -3175,237 +3177,237 @@
     </row>
     <row r="8" spans="1:83" ht="17.25" customHeight="1">
       <c r="A8" s="25"/>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="82" t="s">
+      <c r="G8" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="82" t="s">
+      <c r="H8" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="87" t="s">
+      <c r="I8" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="83"/>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="105" t="s">
+      <c r="J8" s="93"/>
+      <c r="K8" s="93"/>
+      <c r="L8" s="93"/>
+      <c r="M8" s="93"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="93"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="93"/>
+      <c r="U8" s="93"/>
+      <c r="V8" s="93"/>
+      <c r="W8" s="93"/>
+      <c r="X8" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="Y8" s="83"/>
-      <c r="Z8" s="83"/>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="83"/>
-      <c r="AF8" s="83"/>
-      <c r="AG8" s="83"/>
-      <c r="AH8" s="83"/>
-      <c r="AI8" s="83"/>
-      <c r="AJ8" s="83"/>
-      <c r="AK8" s="83"/>
-      <c r="AL8" s="83"/>
-      <c r="AM8" s="104" t="s">
+      <c r="Y8" s="93"/>
+      <c r="Z8" s="93"/>
+      <c r="AA8" s="93"/>
+      <c r="AB8" s="93"/>
+      <c r="AC8" s="93"/>
+      <c r="AD8" s="93"/>
+      <c r="AE8" s="93"/>
+      <c r="AF8" s="93"/>
+      <c r="AG8" s="93"/>
+      <c r="AH8" s="93"/>
+      <c r="AI8" s="93"/>
+      <c r="AJ8" s="93"/>
+      <c r="AK8" s="93"/>
+      <c r="AL8" s="93"/>
+      <c r="AM8" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="AN8" s="83"/>
-      <c r="AO8" s="83"/>
-      <c r="AP8" s="83"/>
-      <c r="AQ8" s="83"/>
-      <c r="AR8" s="83"/>
-      <c r="AS8" s="83"/>
-      <c r="AT8" s="83"/>
-      <c r="AU8" s="83"/>
-      <c r="AV8" s="83"/>
-      <c r="AW8" s="83"/>
-      <c r="AX8" s="83"/>
-      <c r="AY8" s="83"/>
-      <c r="AZ8" s="83"/>
-      <c r="BA8" s="83"/>
-      <c r="BB8" s="101" t="s">
+      <c r="AN8" s="93"/>
+      <c r="AO8" s="93"/>
+      <c r="AP8" s="93"/>
+      <c r="AQ8" s="93"/>
+      <c r="AR8" s="93"/>
+      <c r="AS8" s="93"/>
+      <c r="AT8" s="93"/>
+      <c r="AU8" s="93"/>
+      <c r="AV8" s="93"/>
+      <c r="AW8" s="93"/>
+      <c r="AX8" s="93"/>
+      <c r="AY8" s="93"/>
+      <c r="AZ8" s="93"/>
+      <c r="BA8" s="93"/>
+      <c r="BB8" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="BC8" s="83"/>
-      <c r="BD8" s="83"/>
-      <c r="BE8" s="83"/>
-      <c r="BF8" s="83"/>
-      <c r="BG8" s="83"/>
-      <c r="BH8" s="83"/>
-      <c r="BI8" s="83"/>
-      <c r="BJ8" s="83"/>
-      <c r="BK8" s="83"/>
-      <c r="BL8" s="83"/>
-      <c r="BM8" s="83"/>
-      <c r="BN8" s="83"/>
-      <c r="BO8" s="83"/>
-      <c r="BP8" s="102"/>
-      <c r="BQ8" s="107" t="s">
+      <c r="BC8" s="93"/>
+      <c r="BD8" s="93"/>
+      <c r="BE8" s="93"/>
+      <c r="BF8" s="93"/>
+      <c r="BG8" s="93"/>
+      <c r="BH8" s="93"/>
+      <c r="BI8" s="93"/>
+      <c r="BJ8" s="93"/>
+      <c r="BK8" s="93"/>
+      <c r="BL8" s="93"/>
+      <c r="BM8" s="93"/>
+      <c r="BN8" s="93"/>
+      <c r="BO8" s="93"/>
+      <c r="BP8" s="94"/>
+      <c r="BQ8" s="83" t="s">
         <v>73</v>
       </c>
-      <c r="BR8" s="108"/>
-      <c r="BS8" s="108"/>
-      <c r="BT8" s="108"/>
-      <c r="BU8" s="108"/>
-      <c r="BV8" s="108"/>
-      <c r="BW8" s="108"/>
-      <c r="BX8" s="108"/>
-      <c r="BY8" s="108"/>
-      <c r="BZ8" s="108"/>
-      <c r="CA8" s="108"/>
-      <c r="CB8" s="108"/>
-      <c r="CC8" s="108"/>
-      <c r="CD8" s="108"/>
-      <c r="CE8" s="109"/>
+      <c r="BR8" s="84"/>
+      <c r="BS8" s="84"/>
+      <c r="BT8" s="84"/>
+      <c r="BU8" s="84"/>
+      <c r="BV8" s="84"/>
+      <c r="BW8" s="84"/>
+      <c r="BX8" s="84"/>
+      <c r="BY8" s="84"/>
+      <c r="BZ8" s="84"/>
+      <c r="CA8" s="84"/>
+      <c r="CB8" s="84"/>
+      <c r="CC8" s="84"/>
+      <c r="CD8" s="84"/>
+      <c r="CE8" s="85"/>
     </row>
     <row r="9" spans="1:83" ht="17.25" customHeight="1">
       <c r="A9" s="26"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="84" t="s">
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="84" t="s">
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="84" t="s">
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="90"/>
+      <c r="R9" s="91"/>
+      <c r="S9" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="T9" s="85"/>
-      <c r="U9" s="85"/>
-      <c r="V9" s="85"/>
-      <c r="W9" s="86"/>
-      <c r="X9" s="103" t="s">
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="91"/>
+      <c r="X9" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="85"/>
-      <c r="AB9" s="86"/>
-      <c r="AC9" s="103" t="s">
+      <c r="Y9" s="90"/>
+      <c r="Z9" s="90"/>
+      <c r="AA9" s="90"/>
+      <c r="AB9" s="91"/>
+      <c r="AC9" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="AD9" s="85"/>
-      <c r="AE9" s="85"/>
-      <c r="AF9" s="85"/>
-      <c r="AG9" s="86"/>
-      <c r="AH9" s="103" t="s">
+      <c r="AD9" s="90"/>
+      <c r="AE9" s="90"/>
+      <c r="AF9" s="90"/>
+      <c r="AG9" s="91"/>
+      <c r="AH9" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="AI9" s="85"/>
-      <c r="AJ9" s="85"/>
-      <c r="AK9" s="85"/>
-      <c r="AL9" s="86"/>
-      <c r="AM9" s="106" t="s">
+      <c r="AI9" s="90"/>
+      <c r="AJ9" s="90"/>
+      <c r="AK9" s="90"/>
+      <c r="AL9" s="91"/>
+      <c r="AM9" s="98" t="s">
         <v>76</v>
       </c>
-      <c r="AN9" s="85"/>
-      <c r="AO9" s="85"/>
-      <c r="AP9" s="85"/>
-      <c r="AQ9" s="86"/>
-      <c r="AR9" s="106" t="s">
+      <c r="AN9" s="90"/>
+      <c r="AO9" s="90"/>
+      <c r="AP9" s="90"/>
+      <c r="AQ9" s="91"/>
+      <c r="AR9" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="AS9" s="85"/>
-      <c r="AT9" s="85"/>
-      <c r="AU9" s="85"/>
-      <c r="AV9" s="86"/>
-      <c r="AW9" s="106" t="s">
+      <c r="AS9" s="90"/>
+      <c r="AT9" s="90"/>
+      <c r="AU9" s="90"/>
+      <c r="AV9" s="91"/>
+      <c r="AW9" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="AX9" s="85"/>
-      <c r="AY9" s="85"/>
-      <c r="AZ9" s="85"/>
-      <c r="BA9" s="86"/>
-      <c r="BB9" s="100" t="s">
+      <c r="AX9" s="90"/>
+      <c r="AY9" s="90"/>
+      <c r="AZ9" s="90"/>
+      <c r="BA9" s="91"/>
+      <c r="BB9" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="BC9" s="85"/>
-      <c r="BD9" s="85"/>
-      <c r="BE9" s="85"/>
-      <c r="BF9" s="86"/>
-      <c r="BG9" s="100" t="s">
+      <c r="BC9" s="90"/>
+      <c r="BD9" s="90"/>
+      <c r="BE9" s="90"/>
+      <c r="BF9" s="91"/>
+      <c r="BG9" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="BH9" s="85"/>
-      <c r="BI9" s="85"/>
-      <c r="BJ9" s="85"/>
-      <c r="BK9" s="86"/>
-      <c r="BL9" s="100" t="s">
+      <c r="BH9" s="90"/>
+      <c r="BI9" s="90"/>
+      <c r="BJ9" s="90"/>
+      <c r="BK9" s="91"/>
+      <c r="BL9" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="BM9" s="85"/>
-      <c r="BN9" s="85"/>
-      <c r="BO9" s="85"/>
-      <c r="BP9" s="86"/>
-      <c r="BQ9" s="110" t="s">
+      <c r="BM9" s="90"/>
+      <c r="BN9" s="90"/>
+      <c r="BO9" s="90"/>
+      <c r="BP9" s="91"/>
+      <c r="BQ9" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="BR9" s="111"/>
-      <c r="BS9" s="111"/>
-      <c r="BT9" s="111"/>
-      <c r="BU9" s="112"/>
-      <c r="BV9" s="110" t="s">
+      <c r="BR9" s="87"/>
+      <c r="BS9" s="87"/>
+      <c r="BT9" s="87"/>
+      <c r="BU9" s="88"/>
+      <c r="BV9" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="BW9" s="111"/>
-      <c r="BX9" s="111"/>
-      <c r="BY9" s="111"/>
-      <c r="BZ9" s="112"/>
-      <c r="CA9" s="110" t="s">
+      <c r="BW9" s="87"/>
+      <c r="BX9" s="87"/>
+      <c r="BY9" s="87"/>
+      <c r="BZ9" s="88"/>
+      <c r="CA9" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="CB9" s="111"/>
-      <c r="CC9" s="111"/>
-      <c r="CD9" s="111"/>
-      <c r="CE9" s="112"/>
+      <c r="CB9" s="87"/>
+      <c r="CC9" s="87"/>
+      <c r="CD9" s="87"/>
+      <c r="CE9" s="88"/>
     </row>
     <row r="10" spans="1:83" ht="17.25" customHeight="1">
       <c r="A10" s="27"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="93"/>
       <c r="I10" s="36" t="s">
         <v>20</v>
       </c>
@@ -6456,11 +6458,11 @@
       <c r="BN38" s="50"/>
       <c r="BO38" s="79"/>
       <c r="BP38" s="79"/>
-      <c r="BQ38" s="113"/>
-      <c r="BR38" s="113"/>
-      <c r="BS38" s="113"/>
-      <c r="BT38" s="113"/>
-      <c r="BU38" s="113"/>
+      <c r="BQ38" s="82"/>
+      <c r="BR38" s="82"/>
+      <c r="BS38" s="82"/>
+      <c r="BT38" s="82"/>
+      <c r="BU38" s="82"/>
       <c r="BV38" s="56"/>
       <c r="BW38" s="56"/>
       <c r="BX38" s="56"/>
@@ -6561,15 +6563,17 @@
       <c r="BS39" s="57"/>
       <c r="BT39" s="57"/>
       <c r="BU39" s="57"/>
-      <c r="BV39" s="72" t="s">
+      <c r="BV39" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="BW39" s="72" t="s">
+      <c r="BW39" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="BX39" s="63"/>
-      <c r="BY39" s="113"/>
-      <c r="BZ39" s="113"/>
+      <c r="BX39" s="114" t="s">
+        <v>35</v>
+      </c>
+      <c r="BY39" s="82"/>
+      <c r="BZ39" s="82"/>
       <c r="CA39" s="57"/>
       <c r="CB39" s="57"/>
       <c r="CC39" s="57"/>
@@ -6791,12 +6795,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="BQ8:CE8"/>
-    <mergeCell ref="BQ9:BU9"/>
-    <mergeCell ref="BV9:BZ9"/>
-    <mergeCell ref="CA9:CE9"/>
-    <mergeCell ref="BG9:BK9"/>
-    <mergeCell ref="BL9:BP9"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="P5:AA5"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="O2:AG2"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="BB9:BF9"/>
     <mergeCell ref="BB8:BP8"/>
     <mergeCell ref="X9:AB9"/>
@@ -6807,28 +6827,12 @@
     <mergeCell ref="AR9:AV9"/>
     <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="P5:AA5"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="O2:AG2"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="BQ8:CE8"/>
+    <mergeCell ref="BQ9:BU9"/>
+    <mergeCell ref="BV9:BZ9"/>
+    <mergeCell ref="CA9:CE9"/>
+    <mergeCell ref="BG9:BK9"/>
+    <mergeCell ref="BL9:BP9"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <conditionalFormatting sqref="K14">

</xml_diff>